<commit_message>
notes for next time
</commit_message>
<xml_diff>
--- a/05_results/results_tables/AIC_all_2025.xlsx
+++ b/05_results/results_tables/AIC_all_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uqasmi57/Documents/Offline_Projects/rare_reptiles/05_results/results_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8C8F3A-3D77-7C43-95B4-66E20339920A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE2B0C1-0445-8F49-9EE4-B65E04502151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="600" windowWidth="22840" windowHeight="13720" xr2:uid="{C0406F75-2846-534A-B1C3-50466FB156C3}"/>
   </bookViews>
@@ -959,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7EA48B-B8F7-8742-83D2-9F74DF941AD4}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>